<commit_message>
Start Fires During Fire Seas
Reintroduce fire probability after node is reborn and give chance for node to catch fire
</commit_message>
<xml_diff>
--- a/CaliforniaCountyList.xlsx
+++ b/CaliforniaCountyList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarte\Documents\Github\CMPLXSYS530\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D496D965-2F57-4A17-8A8B-E6EF52A86FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3C6FDF-295D-4FDA-AA51-08600E8B370E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{224B5DCA-8CFB-4388-A88F-750FC01ACBFD}"/>
+    <workbookView xWindow="14370" yWindow="1608" windowWidth="17280" windowHeight="10074" xr2:uid="{224B5DCA-8CFB-4388-A88F-750FC01ACBFD}"/>
   </bookViews>
   <sheets>
     <sheet name="County Data" sheetId="1" r:id="rId1"/>
@@ -980,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BE8DAF-C69E-4C2C-A52C-E34A800ED6B8}">
   <dimension ref="A1:AA59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>